<commit_message>
Add third school example
</commit_message>
<xml_diff>
--- a/inst/extdata/school.xlsx
+++ b/inst/extdata/school.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
   <si>
     <t xml:space="preserve">% Proficient or Higher</t>
   </si>
@@ -231,20 +232,103 @@
   </si>
   <si>
     <t xml:space="preserve">Grade 09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUDENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATOR EXPERIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATOR QUALIFICATIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years w/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years in MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-SEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endorsed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State (All Students)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0"/>
     <numFmt numFmtId="168" formatCode="#,##0%;\-#,##0%;&quot;0 &quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0%;\-#,##0.0%;&quot;0 &quot;"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -320,8 +404,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,7 +435,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E5E5"/>
-        <bgColor rgb="FFE7E7E7"/>
+        <bgColor rgb="FFE5E5E5"/>
       </patternFill>
     </fill>
     <fill>
@@ -352,8 +444,14 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFE7E7E7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="21">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -453,6 +551,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFE5E5E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE5E5E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE5E5E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE5E5E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FFE2E2E2"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE2E2E2"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE2E2E2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE2E2E2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -479,7 +723,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,6 +817,130 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,13 +988,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE7E5E5"/>
+      <rgbColor rgb="FFE5E5E5"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFE2E2E2"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -2118,7 +2486,7 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2410,4 +2778,337 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="7.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="30"/>
+      <c r="K3" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="30"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="42"/>
+      <c r="L6" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="44" t="n">
+        <v>738499</v>
+      </c>
+      <c r="C7" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="46" t="n">
+        <v>0.842777337106</v>
+      </c>
+      <c r="E7" s="46" t="n">
+        <v>0.103685079428</v>
+      </c>
+      <c r="F7" s="46" t="n">
+        <v>0.053537583465</v>
+      </c>
+      <c r="G7" s="47" t="n">
+        <v>0.753081989829</v>
+      </c>
+      <c r="H7" s="46" t="n">
+        <v>0.24691801017</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>0.01116516719</v>
+      </c>
+      <c r="J7" s="47" t="n">
+        <v>0.903456339044</v>
+      </c>
+      <c r="K7" s="47" t="n">
+        <v>0.096543660955</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="44" t="n">
+        <v>625</v>
+      </c>
+      <c r="C8" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="46" t="n">
+        <v>0.896170212765</v>
+      </c>
+      <c r="E8" s="46" t="n">
+        <v>0.059939209726</v>
+      </c>
+      <c r="F8" s="46" t="n">
+        <v>0.043890577507</v>
+      </c>
+      <c r="G8" s="47" t="n">
+        <v>0.752102376599</v>
+      </c>
+      <c r="H8" s="46" t="n">
+        <v>0.2478976234</v>
+      </c>
+      <c r="I8" s="46" t="n">
+        <v>0.001823708206</v>
+      </c>
+      <c r="J8" s="47" t="n">
+        <v>0.944437689969</v>
+      </c>
+      <c r="K8" s="47" t="n">
+        <v>0.05556231003</v>
+      </c>
+      <c r="L8" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" s="48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="50" t="n">
+        <v>116</v>
+      </c>
+      <c r="C9" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="52" t="n">
+        <v>0.846153846153</v>
+      </c>
+      <c r="E9" s="52" t="n">
+        <v>0.153846153846</v>
+      </c>
+      <c r="F9" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="53" t="n">
+        <v>0.931623931623</v>
+      </c>
+      <c r="H9" s="52" t="n">
+        <v>0.068376068376</v>
+      </c>
+      <c r="I9" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D4:F4"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>